<commit_message>
Updated pulse shaping extension production files
</commit_message>
<xml_diff>
--- a/schematics/kicad/pulse-shaping-extension-v1.1/production/pulse-shaping-extension-v1.1-BOM.xlsx
+++ b/schematics/kicad/pulse-shaping-extension-v1.1/production/pulse-shaping-extension-v1.1-BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>Comment</t>
   </si>
@@ -49,7 +49,7 @@
     <t>C653184</t>
   </si>
   <si>
-    <t>OB3225125MLDB6SI-00</t>
+    <t>CO32D6-125.000-33GDTSTL</t>
   </si>
   <si>
     <t>X1</t>
@@ -58,7 +58,7 @@
     <t>SMD3225-6P</t>
   </si>
   <si>
-    <t>C5173622</t>
+    <t>C5119019</t>
   </si>
   <si>
     <t>100Ω</t>
@@ -157,16 +157,16 @@
     <t>C5422</t>
   </si>
   <si>
-    <t>ADM8829ARTZ-REEL7</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
-    <t>C658578</t>
+    <t>MAX1853EXT+T</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-363-6</t>
+  </si>
+  <si>
+    <t>C143384</t>
   </si>
   <si>
     <t>560Ω</t>
@@ -175,10 +175,16 @@
     <t>R11</t>
   </si>
   <si>
+    <t>C23204</t>
+  </si>
+  <si>
     <t>120Ω</t>
   </si>
   <si>
     <t>R12</t>
+  </si>
+  <si>
+    <t>C22787</t>
   </si>
   <si>
     <t>DNP</t>
@@ -1690,26 +1696,30 @@
       <c r="C16" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" t="s" s="4">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" ht="14.7" customHeight="1">
       <c r="A17" t="s" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s" s="5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" t="s" s="4">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" ht="14.7" customHeight="1">
       <c r="A18" t="s" s="4">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s" s="4">
         <v>21</v>
@@ -1718,44 +1728,44 @@
     </row>
     <row r="19" ht="14.7" customHeight="1">
       <c r="A19" t="s" s="4">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s" s="4">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" ht="14.7" customHeight="1">
       <c r="A20" t="s" s="4">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s" s="4">
         <v>6</v>
       </c>
       <c r="D20" t="s" s="4">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" ht="14.7" customHeight="1">
       <c r="A21" t="s" s="4">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s" s="4">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s" s="4">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" ht="14.7" customHeight="1">
@@ -1763,83 +1773,83 @@
         <v>29</v>
       </c>
       <c r="B22" t="s" s="6">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s" s="4">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s" s="4">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" ht="14.7" customHeight="1">
       <c r="A23" t="s" s="4">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s" s="5">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s" s="4">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s" s="4">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" ht="14.7" customHeight="1">
       <c r="A24" t="s" s="4">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s" s="5">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s" s="4">
         <v>46</v>
       </c>
       <c r="D24" t="s" s="4">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" ht="14.7" customHeight="1">
       <c r="A25" t="s" s="4">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s" s="4">
         <v>6</v>
       </c>
       <c r="D25" t="s" s="4">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" ht="14.7" customHeight="1">
       <c r="A26" t="s" s="4">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s" s="4">
         <v>6</v>
       </c>
       <c r="D26" t="s" s="4">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" ht="14.7" customHeight="1">
       <c r="A27" t="s" s="4">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s" s="5">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s" s="4">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>